<commit_message>
change in component list
</commit_message>
<xml_diff>
--- a/Components/component list.xlsx
+++ b/Components/component list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>SL NO</t>
   </si>
@@ -82,12 +82,6 @@
   </si>
   <si>
     <t>For connections</t>
-  </si>
-  <si>
-    <t>SMPS</t>
-  </si>
-  <si>
-    <t>For powering the system</t>
   </si>
 </sst>
 </file>
@@ -405,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,20 +537,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>